<commit_message>
Bug and code format fixed.
</commit_message>
<xml_diff>
--- a/PCR_Bot_Template.xlsx
+++ b/PCR_Bot_Template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\University\Code\PY\PCR_Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9343FF04-B198-4778-8A45-ACB6F7CE7CB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB041E2D-D1CE-4DE4-8D73-9AB218A6DEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Boss" sheetId="2" r:id="rId1"/>
-    <sheet name="Template" sheetId="1" r:id="rId2"/>
+    <sheet name="Boss" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,6 +31,21 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
+    <t>飞龙</t>
+  </si>
+  <si>
+    <t>狂暴格里芬</t>
+  </si>
+  <si>
+    <t>兽人酋长</t>
+  </si>
+  <si>
+    <t>圣灵角鹿</t>
+  </si>
+  <si>
+    <t>牛头怪</t>
+  </si>
+  <si>
     <t xml:space="preserve">       日期
 刀序</t>
   </si>
@@ -78,26 +93,6 @@
   </si>
   <si>
     <t>涨幅</t>
-  </si>
-  <si>
-    <t>飞龙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>狂暴格里芬</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>兽人酋长</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣灵角鹿</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>牛头怪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -353,7 +348,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7340-4F16-A8D5-02F70AD6C8E6}"/>
+              <c16:uniqueId val="{00000000-54C8-45AB-8F39-98AF167AEDE9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -424,7 +419,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7340-4F16-A8D5-02F70AD6C8E6}"/>
+              <c16:uniqueId val="{00000001-54C8-45AB-8F39-98AF167AEDE9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -495,7 +490,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7340-4F16-A8D5-02F70AD6C8E6}"/>
+              <c16:uniqueId val="{00000002-54C8-45AB-8F39-98AF167AEDE9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -537,7 +532,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7340-4F16-A8D5-02F70AD6C8E6}"/>
+              <c16:uniqueId val="{00000003-54C8-45AB-8F39-98AF167AEDE9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -724,7 +719,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1041,21 +1036,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3CF3A3-681F-48BC-A676-4627A984E22F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>6000000</v>
@@ -1063,7 +1058,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>8000000</v>
@@ -1071,7 +1066,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>10000000</v>
@@ -1079,7 +1074,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>12000000</v>
@@ -1087,7 +1082,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>20000000</v>
@@ -1096,15 +1091,15 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -1121,33 +1116,33 @@
     </row>
     <row r="3" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1159,7 +1154,7 @@
     </row>
     <row r="5" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1169,7 +1164,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="K5" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L5" s="4">
         <v>0</v>
@@ -1177,7 +1172,7 @@
     </row>
     <row r="6" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1187,7 +1182,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="K6" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -1195,7 +1190,7 @@
     </row>
     <row r="7" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1207,7 +1202,7 @@
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1219,7 +1214,7 @@
     </row>
     <row r="9" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1231,7 +1226,7 @@
     </row>
     <row r="10" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" ref="C10:I10" si="0">SUM(C5,C7,C9)</f>
@@ -1264,7 +1259,7 @@
     </row>
     <row r="11" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="e">

</xml_diff>

<commit_message>
Compensate time system bugs fixed & speed up & some functions rebuilt.
</commit_message>
<xml_diff>
--- a/PCR_Bot_Template.xlsx
+++ b/PCR_Bot_Template.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\University\Code\PY\PCR_Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\University\Code\PY\PCR_Bot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB041E2D-D1CE-4DE4-8D73-9AB218A6DEAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F56DAC9-7C4E-463B-B854-3230F09E830C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Boss" sheetId="1" r:id="rId1"/>
-    <sheet name="Template" sheetId="2" r:id="rId2"/>
+    <sheet name="Boss" sheetId="2" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,22 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
-  <si>
-    <t>飞龙</t>
-  </si>
-  <si>
-    <t>狂暴格里芬</t>
-  </si>
-  <si>
-    <t>兽人酋长</t>
-  </si>
-  <si>
-    <t>圣灵角鹿</t>
-  </si>
-  <si>
-    <t>牛头怪</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="21">
   <si>
     <t xml:space="preserve">       日期
 刀序</t>
@@ -93,6 +78,26 @@
   </si>
   <si>
     <t>涨幅</t>
+  </si>
+  <si>
+    <t>飞龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂暴格里芬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兽人酋长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣灵角鹿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛头怪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -348,7 +353,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-54C8-45AB-8F39-98AF167AEDE9}"/>
+              <c16:uniqueId val="{00000000-7340-4F16-A8D5-02F70AD6C8E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -419,7 +424,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-54C8-45AB-8F39-98AF167AEDE9}"/>
+              <c16:uniqueId val="{00000001-7340-4F16-A8D5-02F70AD6C8E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -490,7 +495,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-54C8-45AB-8F39-98AF167AEDE9}"/>
+              <c16:uniqueId val="{00000002-7340-4F16-A8D5-02F70AD6C8E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -532,7 +537,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-54C8-45AB-8F39-98AF167AEDE9}"/>
+              <c16:uniqueId val="{00000003-7340-4F16-A8D5-02F70AD6C8E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -719,7 +724,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1036,70 +1041,580 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3CF3A3-681F-48BC-A676-4627A984E22F}">
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1">
         <v>6000000</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>8000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>12000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>20000000</v>
+      </c>
+      <c r="C5">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>6000000</v>
+      </c>
+      <c r="C6">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>8000000</v>
+      </c>
+      <c r="C7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>10000000</v>
+      </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>12000000</v>
+      </c>
+      <c r="C9">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>20000000</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>6000000</v>
+      </c>
+      <c r="C11">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>8000000</v>
+      </c>
+      <c r="C12">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>10000000</v>
+      </c>
+      <c r="C13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>12000000</v>
+      </c>
+      <c r="C14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>20000000</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>6000000</v>
+      </c>
+      <c r="C16">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>8000000</v>
+      </c>
+      <c r="C17">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>10000000</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>12000000</v>
+      </c>
+      <c r="C19">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>20000000</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>6000000</v>
+      </c>
+      <c r="C21">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>8000000</v>
+      </c>
+      <c r="C22">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>10000000</v>
+      </c>
+      <c r="C23">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>12000000</v>
+      </c>
+      <c r="C24">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>20000000</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>6000000</v>
+      </c>
+      <c r="C26">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>8000000</v>
+      </c>
+      <c r="C27">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>10000000</v>
+      </c>
+      <c r="C28">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>12000000</v>
+      </c>
+      <c r="C29">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>20000000</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>6000000</v>
+      </c>
+      <c r="C31">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <v>8000000</v>
+      </c>
+      <c r="C32">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>10000000</v>
+      </c>
+      <c r="C33">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>12000000</v>
+      </c>
+      <c r="C34">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>20000000</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>6000000</v>
+      </c>
+      <c r="C36">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37">
+        <v>8000000</v>
+      </c>
+      <c r="C37">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38">
+        <v>10000000</v>
+      </c>
+      <c r="C38">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39">
+        <v>12000000</v>
+      </c>
+      <c r="C39">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>20000000</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41">
+        <v>6000000</v>
+      </c>
+      <c r="C41">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>8000000</v>
+      </c>
+      <c r="C42">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43">
+        <v>10000000</v>
+      </c>
+      <c r="C43">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44">
+        <v>12000000</v>
+      </c>
+      <c r="C44">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>20000000</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>6000000</v>
+      </c>
+      <c r="C46">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47">
+        <v>8000000</v>
+      </c>
+      <c r="C47">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <v>10000000</v>
+      </c>
+      <c r="C48">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49">
+        <v>12000000</v>
+      </c>
+      <c r="C49">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <v>20000000</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -1116,33 +1631,33 @@
     </row>
     <row r="3" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1154,7 +1669,7 @@
     </row>
     <row r="5" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1164,7 +1679,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="K5" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L5" s="4">
         <v>0</v>
@@ -1172,7 +1687,7 @@
     </row>
     <row r="6" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1182,7 +1697,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="K6" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -1190,7 +1705,7 @@
     </row>
     <row r="7" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1202,7 +1717,7 @@
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1214,7 +1729,7 @@
     </row>
     <row r="9" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1226,7 +1741,7 @@
     </row>
     <row r="10" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" ref="C10:I10" si="0">SUM(C5,C7,C9)</f>
@@ -1259,7 +1774,7 @@
     </row>
     <row r="11" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="e">

</xml_diff>

<commit_message>
Compensate atk time system update.
</commit_message>
<xml_diff>
--- a/PCR_Bot_Template.xlsx
+++ b/PCR_Bot_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\University\Code\PY\PCR_Bot\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\University\Code\PY\PCR_Bot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F56DAC9-7C4E-463B-B854-3230F09E830C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751C5A93-C03B-4F74-A97A-0A944634C555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boss" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t xml:space="preserve">       日期
 刀序</t>
@@ -71,9 +71,6 @@
     <t>第 2 刀</t>
   </si>
   <si>
-    <t>第 3 刀</t>
-  </si>
-  <si>
     <t>总计分数</t>
   </si>
   <si>
@@ -97,6 +94,14 @@
   </si>
   <si>
     <t>牛头怪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阵容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第3刀</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -229,520 +234,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
-              <a:t>分数</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Template!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>第 1 刀</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Template!$C$3:$I$3</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Template!$C$5:$I$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7340-4F16-A8D5-02F70AD6C8E6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Template!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>第 2 刀</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Template!$C$3:$I$3</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Template!$C$7:$I$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7340-4F16-A8D5-02F70AD6C8E6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Template!$B$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>第 3 刀</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Template!$C$3:$I$3</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Template!$C$9:$I$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7340-4F16-A8D5-02F70AD6C8E6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Template!$B$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>总计分数</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7340-4F16-A8D5-02F70AD6C8E6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="619898159"/>
-        <c:axId val="614260527"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="619898159"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="614260527"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="614260527"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="619898159"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>6673</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>84044</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>18675</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>56030</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1044,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3CF3A3-681F-48BC-A676-4627A984E22F}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -1055,7 +546,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1">
         <v>6000000</v>
@@ -1066,7 +557,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>8000000</v>
@@ -1077,7 +568,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>10000000</v>
@@ -1088,7 +579,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>12000000</v>
@@ -1099,7 +590,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>20000000</v>
@@ -1110,7 +601,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>6000000</v>
@@ -1121,7 +612,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>8000000</v>
@@ -1132,7 +623,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>10000000</v>
@@ -1143,7 +634,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>12000000</v>
@@ -1154,7 +645,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>20000000</v>
@@ -1165,7 +656,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>6000000</v>
@@ -1176,7 +667,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>8000000</v>
@@ -1187,7 +678,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>10000000</v>
@@ -1198,7 +689,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>12000000</v>
@@ -1209,7 +700,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>20000000</v>
@@ -1220,7 +711,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>6000000</v>
@@ -1231,7 +722,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>8000000</v>
@@ -1242,7 +733,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>10000000</v>
@@ -1253,7 +744,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>12000000</v>
@@ -1264,7 +755,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>20000000</v>
@@ -1275,7 +766,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>6000000</v>
@@ -1286,7 +777,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>8000000</v>
@@ -1297,7 +788,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>10000000</v>
@@ -1308,7 +799,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>12000000</v>
@@ -1319,7 +810,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25">
         <v>20000000</v>
@@ -1330,7 +821,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26">
         <v>6000000</v>
@@ -1341,7 +832,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27">
         <v>8000000</v>
@@ -1352,7 +843,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28">
         <v>10000000</v>
@@ -1363,7 +854,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29">
         <v>12000000</v>
@@ -1374,7 +865,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30">
         <v>20000000</v>
@@ -1385,7 +876,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31">
         <v>6000000</v>
@@ -1396,7 +887,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32">
         <v>8000000</v>
@@ -1407,7 +898,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33">
         <v>10000000</v>
@@ -1418,7 +909,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34">
         <v>12000000</v>
@@ -1429,7 +920,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35">
         <v>20000000</v>
@@ -1440,7 +931,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36">
         <v>6000000</v>
@@ -1451,7 +942,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37">
         <v>8000000</v>
@@ -1462,7 +953,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38">
         <v>10000000</v>
@@ -1473,7 +964,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39">
         <v>12000000</v>
@@ -1484,7 +975,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40">
         <v>20000000</v>
@@ -1495,7 +986,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41">
         <v>6000000</v>
@@ -1506,7 +997,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42">
         <v>8000000</v>
@@ -1517,7 +1008,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43">
         <v>10000000</v>
@@ -1528,7 +1019,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44">
         <v>12000000</v>
@@ -1539,7 +1030,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45">
         <v>20000000</v>
@@ -1550,7 +1041,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46">
         <v>6000000</v>
@@ -1561,7 +1052,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47">
         <v>8000000</v>
@@ -1572,7 +1063,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48">
         <v>10000000</v>
@@ -1583,7 +1074,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49">
         <v>12000000</v>
@@ -1594,7 +1085,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50">
         <v>20000000</v>
@@ -1614,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1716,8 +1207,8 @@
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="5" t="s">
-        <v>8</v>
+      <c r="B8" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1729,7 +1220,7 @@
     </row>
     <row r="9" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1741,14 +1232,14 @@
     </row>
     <row r="10" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6">
-        <f t="shared" ref="C10:I10" si="0">SUM(C5,C7,C9)</f>
+        <f>SUM(C5,C7,C9)</f>
         <v>0</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D10:I10" si="0">SUM(D5,D7,D9)</f>
         <v>0</v>
       </c>
       <c r="E10" s="6">
@@ -1774,7 +1265,7 @@
     </row>
     <row r="11" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="e">
@@ -1786,7 +1277,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F11" s="6" t="e">
-        <f t="shared" si="1"/>
+        <f>(F10-E10)/E10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G11" s="6" t="e">
@@ -1816,6 +1307,5 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>